<commit_message>
Update business case financials
</commit_message>
<xml_diff>
--- a/1.2 business_case_financials.xlsx
+++ b/1.2 business_case_financials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privacy\ASU_Fall22\CSE441 Software Project Management\Project\MyProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C339AC5-8E6C-4AE1-9486-415E39D81252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04932AD6-9EFF-4A6E-94A6-D5F9006E397B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Costs</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Assumptions</t>
   </si>
   <si>
-    <t>Enter assumptions here</t>
-  </si>
-  <si>
     <t>Date:</t>
   </si>
   <si>
@@ -85,22 +82,37 @@
     <t>Discount rate Year</t>
   </si>
   <si>
-    <t>Discount rate Month</t>
-  </si>
-  <si>
     <t>Assume the project is completed in Year 1</t>
   </si>
   <si>
     <t>Assume the project is completed in Month 12</t>
   </si>
   <si>
-    <t>Payback in Month 7</t>
-  </si>
-  <si>
     <t>Constant inflation rate and staff availability and consistency.</t>
   </si>
   <si>
     <t>Months</t>
+  </si>
+  <si>
+    <t>Payback in Month 6</t>
+  </si>
+  <si>
+    <t>Discount rate based on the current economical status in egypt is going to be 22%</t>
+  </si>
+  <si>
+    <t>Average Costs of Designing a Web app is around 4.5M-5M</t>
+  </si>
+  <si>
+    <t>Cost of Desiging This web publish system is going to be 4.8M</t>
+  </si>
+  <si>
+    <t>Average interest is estimated to be 1.2M</t>
+  </si>
+  <si>
+    <t>Averaage maintainance cost is estimated to be around 200K for 4 months</t>
+  </si>
+  <si>
+    <t>The client has to pay huge start and second huge payment is after seeing the actual working program, Payment will be done in installements.</t>
   </si>
 </sst>
 </file>
@@ -175,7 +187,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -241,8 +253,9 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -255,6 +268,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -279,15 +294,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>724828</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:colOff>257639</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -305,7 +320,7 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipH="1">
-          <a:off x="5591175" y="3162300"/>
+          <a:off x="13074804" y="3031505"/>
           <a:ext cx="276225" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -328,13 +343,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2371725</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -373,16 +388,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>483220</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>18585</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>399587</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>139389</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>483220</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>147753</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>399587</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>101289</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -399,8 +414,8 @@
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
         <a:xfrm flipV="1">
-          <a:off x="9738732" y="3438292"/>
-          <a:ext cx="0" cy="296437"/>
+          <a:off x="7545660" y="3252438"/>
+          <a:ext cx="0" cy="296436"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -772,10 +787,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P24"/>
+  <dimension ref="A1:Q29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="82" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -785,32 +800,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="22.8" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="A1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="9">
         <v>45108</v>
@@ -848,640 +863,708 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="8">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="8">
-        <f>((1+B4)^(1/12))-1</f>
-        <v>1.2445137919713467E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="8"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="B7" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="1"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="13">
+        <v>0</v>
+      </c>
+      <c r="C8" s="14">
+        <v>1</v>
+      </c>
+      <c r="D8" s="14">
+        <v>2</v>
+      </c>
+      <c r="E8" s="14">
+        <v>3</v>
+      </c>
+      <c r="F8" s="14">
+        <v>4</v>
+      </c>
+      <c r="G8" s="14">
+        <v>5</v>
+      </c>
+      <c r="H8" s="14">
+        <v>6</v>
+      </c>
+      <c r="I8" s="14">
+        <v>7</v>
+      </c>
+      <c r="J8" s="14">
+        <v>8</v>
+      </c>
+      <c r="K8" s="14">
+        <v>9</v>
+      </c>
+      <c r="L8" s="14">
+        <v>10</v>
+      </c>
+      <c r="M8" s="14">
+        <v>11</v>
+      </c>
+      <c r="N8" s="14">
+        <v>12</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="13">
+      <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="14">
-        <v>1</v>
-      </c>
-      <c r="D9" s="14">
-        <v>2</v>
-      </c>
-      <c r="E9" s="14">
-        <v>3</v>
-      </c>
-      <c r="F9" s="14">
-        <v>4</v>
-      </c>
-      <c r="G9" s="14">
-        <v>5</v>
-      </c>
-      <c r="H9" s="14">
-        <v>6</v>
-      </c>
-      <c r="I9" s="14">
-        <v>7</v>
-      </c>
-      <c r="J9" s="14">
-        <v>8</v>
-      </c>
-      <c r="K9" s="14">
-        <v>9</v>
-      </c>
-      <c r="L9" s="14">
-        <v>10</v>
-      </c>
-      <c r="M9" s="14">
-        <v>11</v>
-      </c>
-      <c r="N9" s="14">
-        <v>12</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>8</v>
-      </c>
+      <c r="B9" s="16">
+        <v>1290000</v>
+      </c>
+      <c r="C9" s="16">
+        <v>150000</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1170000</v>
+      </c>
+      <c r="E9" s="16">
+        <v>190000</v>
+      </c>
+      <c r="F9" s="16">
+        <v>111000</v>
+      </c>
+      <c r="G9" s="16">
+        <v>900000</v>
+      </c>
+      <c r="H9" s="16">
+        <v>150000</v>
+      </c>
+      <c r="I9" s="16">
+        <v>200000</v>
+      </c>
+      <c r="J9" s="16">
+        <v>200000</v>
+      </c>
+      <c r="K9" s="16">
+        <v>200000</v>
+      </c>
+      <c r="L9" s="16">
+        <v>200000</v>
+      </c>
+      <c r="M9" s="16">
+        <v>200000</v>
+      </c>
+      <c r="N9" s="16">
+        <v>200000</v>
+      </c>
+      <c r="O9" s="17"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="16">
-        <v>290000</v>
-      </c>
-      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="B10" s="18">
+        <f>B14</f>
+        <v>1</v>
+      </c>
+      <c r="C10" s="18">
+        <f>ROUND(1/(1+$B4)^(C8/12),2)</f>
+        <v>0.98</v>
+      </c>
+      <c r="D10" s="18">
+        <f>ROUND(1/(1+$B4)^(D8/12),2)</f>
+        <v>0.97</v>
+      </c>
+      <c r="E10" s="18">
+        <f>ROUND(1/(1+$B4)^(E8/12),2)</f>
+        <v>0.95</v>
+      </c>
+      <c r="F10" s="18">
+        <f>ROUND(1/(1+$B4)^(F8/12),2)</f>
+        <v>0.94</v>
+      </c>
+      <c r="G10" s="18">
+        <f>ROUND(1/(1+$B4)^(G8/12),2)</f>
+        <v>0.92</v>
+      </c>
+      <c r="H10" s="18">
+        <f>ROUND(1/(1+$B4)^(H8/12),2)</f>
+        <v>0.91</v>
+      </c>
+      <c r="I10" s="18">
+        <f>ROUND(1/(1+$B4)^(I8/12),2)</f>
+        <v>0.89</v>
+      </c>
+      <c r="J10" s="18">
+        <f>ROUND(1/(1+$B4)^(J8/12),2)</f>
+        <v>0.88</v>
+      </c>
+      <c r="K10" s="18">
+        <f>ROUND(1/(1+$B4)^(K8/12),2)</f>
+        <v>0.86</v>
+      </c>
+      <c r="L10" s="18">
+        <f>ROUND(1/(1+$B4)^(L8/12),2)</f>
+        <v>0.85</v>
+      </c>
+      <c r="M10" s="18">
+        <f>ROUND(1/(1+$B4)^(M8/12),2)</f>
+        <v>0.83</v>
+      </c>
+      <c r="N10" s="18">
+        <f>ROUND(1/(1+$B4)^(N8/12),2)</f>
+        <v>0.82</v>
+      </c>
+      <c r="O10" s="17"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="19">
+        <f>B9*B10</f>
+        <v>1290000</v>
+      </c>
+      <c r="C11" s="19">
+        <f>C9*C10</f>
+        <v>147000</v>
+      </c>
+      <c r="D11" s="19">
+        <f>D9*D10</f>
+        <v>1134900</v>
+      </c>
+      <c r="E11" s="19">
+        <f t="shared" ref="E11:M11" si="0">E9*E10</f>
+        <v>180500</v>
+      </c>
+      <c r="F11" s="19">
+        <f t="shared" si="0"/>
+        <v>104340</v>
+      </c>
+      <c r="G11" s="19">
+        <f t="shared" si="0"/>
+        <v>828000</v>
+      </c>
+      <c r="H11" s="19">
+        <f t="shared" si="0"/>
+        <v>136500</v>
+      </c>
+      <c r="I11" s="19">
+        <f t="shared" si="0"/>
+        <v>178000</v>
+      </c>
+      <c r="J11" s="19">
+        <f t="shared" si="0"/>
+        <v>176000</v>
+      </c>
+      <c r="K11" s="19">
+        <f t="shared" si="0"/>
+        <v>172000</v>
+      </c>
+      <c r="L11" s="19">
+        <f t="shared" si="0"/>
+        <v>170000</v>
+      </c>
+      <c r="M11" s="19">
+        <f t="shared" si="0"/>
+        <v>166000</v>
+      </c>
+      <c r="N11" s="19">
+        <f>N9*N10</f>
+        <v>164000</v>
+      </c>
+      <c r="O11" s="20">
+        <f>SUM(B11:N11)</f>
+        <v>4847240</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+      <c r="O12" s="17"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="21">
+        <v>1200000</v>
+      </c>
+      <c r="C13" s="21">
         <v>50000</v>
       </c>
-      <c r="D10" s="16">
-        <v>170000</v>
-      </c>
-      <c r="E10" s="16">
-        <v>90000</v>
-      </c>
-      <c r="F10" s="16">
-        <v>110000</v>
-      </c>
-      <c r="G10" s="16">
-        <v>90000</v>
-      </c>
-      <c r="H10" s="16">
-        <v>150000</v>
-      </c>
-      <c r="I10" s="16">
-        <v>20000</v>
-      </c>
-      <c r="J10" s="16">
-        <v>20000</v>
-      </c>
-      <c r="K10" s="16">
-        <v>20000</v>
-      </c>
-      <c r="L10" s="16">
-        <v>20000</v>
-      </c>
-      <c r="M10" s="16">
-        <v>20000</v>
-      </c>
-      <c r="N10" s="16">
-        <v>20000</v>
-      </c>
-      <c r="O10" s="17"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="18">
-        <f>ROUND(1/(1+$B$5)^B$9,2)</f>
-        <v>1</v>
-      </c>
-      <c r="C11" s="18">
-        <f t="shared" ref="C11:N11" si="0">ROUND(1/(1+$B$5)^C$9,2)</f>
-        <v>0.99</v>
-      </c>
-      <c r="D11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.98</v>
-      </c>
-      <c r="E11" s="18">
-        <f>ROUND(1/(1+$B$5)^E$9,2)</f>
-        <v>0.96</v>
-      </c>
-      <c r="F11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.95</v>
-      </c>
-      <c r="G11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.94</v>
-      </c>
-      <c r="H11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.93</v>
-      </c>
-      <c r="I11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.92</v>
-      </c>
-      <c r="J11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.91</v>
-      </c>
-      <c r="K11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.89</v>
-      </c>
-      <c r="L11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.88</v>
-      </c>
-      <c r="M11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.87</v>
-      </c>
-      <c r="N11" s="18">
-        <f t="shared" si="0"/>
-        <v>0.86</v>
-      </c>
-      <c r="O11" s="17"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="19">
-        <f>B10*B11</f>
-        <v>290000</v>
-      </c>
-      <c r="C12" s="19">
-        <f>C10*C11</f>
-        <v>49500</v>
-      </c>
-      <c r="D12" s="19">
-        <f>D10*D11</f>
-        <v>166600</v>
-      </c>
-      <c r="E12" s="19">
-        <f t="shared" ref="E12:M12" si="1">E10*E11</f>
-        <v>86400</v>
-      </c>
-      <c r="F12" s="19">
-        <f t="shared" si="1"/>
-        <v>104500</v>
-      </c>
-      <c r="G12" s="19">
-        <f t="shared" si="1"/>
-        <v>84600</v>
-      </c>
-      <c r="H12" s="19">
-        <f t="shared" si="1"/>
-        <v>139500</v>
-      </c>
-      <c r="I12" s="19">
-        <f t="shared" si="1"/>
-        <v>18400</v>
-      </c>
-      <c r="J12" s="19">
-        <f t="shared" si="1"/>
-        <v>18200</v>
-      </c>
-      <c r="K12" s="19">
-        <f t="shared" si="1"/>
-        <v>17800</v>
-      </c>
-      <c r="L12" s="19">
-        <f t="shared" si="1"/>
-        <v>17600</v>
-      </c>
-      <c r="M12" s="19">
-        <f t="shared" si="1"/>
-        <v>17400</v>
-      </c>
-      <c r="N12" s="19">
-        <f>N10*N11</f>
-        <v>17200</v>
-      </c>
-      <c r="O12" s="20">
-        <f>SUM(B12:N12)</f>
-        <v>1027700</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
+      <c r="D13" s="21">
+        <v>500000</v>
+      </c>
+      <c r="E13" s="21">
+        <v>140000</v>
+      </c>
+      <c r="F13" s="21">
+        <v>14000</v>
+      </c>
+      <c r="G13" s="21">
+        <v>140000</v>
+      </c>
+      <c r="H13" s="21">
+        <v>1400000</v>
+      </c>
+      <c r="I13" s="21">
+        <v>1900000</v>
+      </c>
+      <c r="J13" s="21">
+        <v>1900000</v>
+      </c>
+      <c r="K13" s="21">
+        <v>1200000</v>
+      </c>
+      <c r="L13" s="21">
+        <v>1250000</v>
+      </c>
+      <c r="M13" s="21">
+        <v>1250000</v>
+      </c>
+      <c r="N13" s="21">
+        <v>1250000</v>
+      </c>
       <c r="O13" s="17"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="21">
-        <v>400000</v>
-      </c>
-      <c r="C14" s="21">
-        <v>50000</v>
-      </c>
-      <c r="D14" s="21">
-        <v>50000</v>
-      </c>
-      <c r="E14" s="21">
-        <v>40000</v>
-      </c>
-      <c r="F14" s="21">
-        <v>40000</v>
-      </c>
-      <c r="G14" s="21">
-        <v>40000</v>
-      </c>
-      <c r="H14" s="21">
-        <v>40000</v>
-      </c>
-      <c r="I14" s="21">
-        <v>90000</v>
-      </c>
-      <c r="J14" s="21">
-        <v>90000</v>
-      </c>
-      <c r="K14" s="21">
-        <v>200000</v>
-      </c>
-      <c r="L14" s="21">
-        <v>250000</v>
-      </c>
-      <c r="M14" s="21">
-        <v>250000</v>
-      </c>
-      <c r="N14" s="21">
-        <v>250000</v>
+        <v>1</v>
+      </c>
+      <c r="B14" s="18">
+        <f>ROUND(1/(1+$B4)^(B8/12),2)</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="18">
+        <f t="shared" ref="C14:N14" si="1">ROUND(1/(1+$B4)^(C8/12),2)</f>
+        <v>0.98</v>
+      </c>
+      <c r="D14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.97</v>
+      </c>
+      <c r="E14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="F14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.94</v>
+      </c>
+      <c r="G14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.92</v>
+      </c>
+      <c r="H14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.91</v>
+      </c>
+      <c r="I14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.89</v>
+      </c>
+      <c r="J14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.88</v>
+      </c>
+      <c r="K14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.86</v>
+      </c>
+      <c r="L14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.85</v>
+      </c>
+      <c r="M14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.83</v>
+      </c>
+      <c r="N14" s="18">
+        <f t="shared" si="1"/>
+        <v>0.82</v>
       </c>
       <c r="O14" s="17"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="18">
-        <f>ROUND(1/(1+$B$5)^B$9,2)</f>
-        <v>1</v>
-      </c>
-      <c r="C15" s="18">
-        <f t="shared" ref="C15:N15" si="2">ROUND(1/(1+$B$5)^C$9,2)</f>
-        <v>0.99</v>
-      </c>
-      <c r="D15" s="18">
+      <c r="A15" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="22">
+        <f>B13*B14</f>
+        <v>1200000</v>
+      </c>
+      <c r="C15" s="22">
+        <f t="shared" ref="C15:M15" si="2">C13*C14</f>
+        <v>49000</v>
+      </c>
+      <c r="D15" s="22">
         <f t="shared" si="2"/>
-        <v>0.98</v>
-      </c>
-      <c r="E15" s="18">
+        <v>485000</v>
+      </c>
+      <c r="E15" s="22">
         <f t="shared" si="2"/>
-        <v>0.96</v>
-      </c>
-      <c r="F15" s="18">
+        <v>133000</v>
+      </c>
+      <c r="F15" s="22">
         <f t="shared" si="2"/>
-        <v>0.95</v>
-      </c>
-      <c r="G15" s="18">
+        <v>13160</v>
+      </c>
+      <c r="G15" s="22">
         <f t="shared" si="2"/>
-        <v>0.94</v>
-      </c>
-      <c r="H15" s="18">
+        <v>128800</v>
+      </c>
+      <c r="H15" s="22">
         <f t="shared" si="2"/>
-        <v>0.93</v>
-      </c>
-      <c r="I15" s="18">
+        <v>1274000</v>
+      </c>
+      <c r="I15" s="22">
         <f t="shared" si="2"/>
-        <v>0.92</v>
-      </c>
-      <c r="J15" s="18">
+        <v>1691000</v>
+      </c>
+      <c r="J15" s="22">
         <f t="shared" si="2"/>
-        <v>0.91</v>
-      </c>
-      <c r="K15" s="18">
+        <v>1672000</v>
+      </c>
+      <c r="K15" s="22">
         <f t="shared" si="2"/>
-        <v>0.89</v>
-      </c>
-      <c r="L15" s="18">
+        <v>1032000</v>
+      </c>
+      <c r="L15" s="22">
         <f t="shared" si="2"/>
-        <v>0.88</v>
-      </c>
-      <c r="M15" s="18">
+        <v>1062500</v>
+      </c>
+      <c r="M15" s="22">
         <f t="shared" si="2"/>
-        <v>0.87</v>
-      </c>
-      <c r="N15" s="18">
-        <f t="shared" si="2"/>
-        <v>0.86</v>
-      </c>
-      <c r="O15" s="17"/>
+        <v>1037500</v>
+      </c>
+      <c r="N15" s="19">
+        <f>N13*N14</f>
+        <v>1024999.9999999999</v>
+      </c>
+      <c r="O15" s="19">
+        <f>SUM(B15:N15)</f>
+        <v>10802960</v>
+      </c>
+      <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="22">
-        <f>B14*B15</f>
-        <v>400000</v>
-      </c>
-      <c r="C16" s="22">
-        <f t="shared" ref="C16:M16" si="3">C14*C15</f>
-        <v>49500</v>
-      </c>
-      <c r="D16" s="22">
+      <c r="A16" s="5"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+      <c r="O16" s="17"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="23">
+        <f>B15-B11</f>
+        <v>-90000</v>
+      </c>
+      <c r="C17" s="23">
+        <f t="shared" ref="C17:M17" si="3">C15-C11</f>
+        <v>-98000</v>
+      </c>
+      <c r="D17" s="23">
         <f t="shared" si="3"/>
-        <v>49000</v>
-      </c>
-      <c r="E16" s="22">
+        <v>-649900</v>
+      </c>
+      <c r="E17" s="23">
         <f t="shared" si="3"/>
-        <v>38400</v>
-      </c>
-      <c r="F16" s="22">
+        <v>-47500</v>
+      </c>
+      <c r="F17" s="23">
         <f t="shared" si="3"/>
-        <v>38000</v>
-      </c>
-      <c r="G16" s="22">
+        <v>-91180</v>
+      </c>
+      <c r="G17" s="23">
         <f t="shared" si="3"/>
-        <v>37600</v>
-      </c>
-      <c r="H16" s="22">
+        <v>-699200</v>
+      </c>
+      <c r="H17" s="23">
         <f t="shared" si="3"/>
-        <v>37200</v>
-      </c>
-      <c r="I16" s="22">
+        <v>1137500</v>
+      </c>
+      <c r="I17" s="23">
         <f t="shared" si="3"/>
-        <v>82800</v>
-      </c>
-      <c r="J16" s="22">
+        <v>1513000</v>
+      </c>
+      <c r="J17" s="23">
         <f t="shared" si="3"/>
-        <v>81900</v>
-      </c>
-      <c r="K16" s="22">
+        <v>1496000</v>
+      </c>
+      <c r="K17" s="23">
         <f t="shared" si="3"/>
-        <v>178000</v>
-      </c>
-      <c r="L16" s="22">
+        <v>860000</v>
+      </c>
+      <c r="L17" s="23">
         <f t="shared" si="3"/>
-        <v>220000</v>
-      </c>
-      <c r="M16" s="22">
+        <v>892500</v>
+      </c>
+      <c r="M17" s="23">
         <f t="shared" si="3"/>
-        <v>217500</v>
-      </c>
-      <c r="N16" s="19">
-        <f>N14*N15</f>
-        <v>215000</v>
-      </c>
-      <c r="O16" s="19">
-        <f>SUM(B16:N16)</f>
-        <v>1644900</v>
-      </c>
-      <c r="P16" s="2" t="s">
+        <v>871500</v>
+      </c>
+      <c r="N17" s="23">
+        <f>N15-N11</f>
+        <v>860999.99999999988</v>
+      </c>
+      <c r="O17" s="20">
+        <f>O15-O11</f>
+        <v>5955720</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="1"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="23">
-        <f>B16-B12</f>
-        <v>110000</v>
+        <f>B17</f>
+        <v>-90000</v>
       </c>
       <c r="C18" s="23">
-        <f t="shared" ref="C18:M18" si="4">C16-C12</f>
-        <v>0</v>
+        <f t="shared" ref="C18:M18" si="4">C17</f>
+        <v>-98000</v>
       </c>
       <c r="D18" s="23">
         <f t="shared" si="4"/>
-        <v>-117600</v>
+        <v>-649900</v>
       </c>
       <c r="E18" s="23">
         <f t="shared" si="4"/>
-        <v>-48000</v>
+        <v>-47500</v>
       </c>
       <c r="F18" s="23">
         <f t="shared" si="4"/>
-        <v>-66500</v>
+        <v>-91180</v>
       </c>
       <c r="G18" s="23">
         <f t="shared" si="4"/>
-        <v>-47000</v>
+        <v>-699200</v>
       </c>
       <c r="H18" s="23">
         <f t="shared" si="4"/>
-        <v>-102300</v>
+        <v>1137500</v>
       </c>
       <c r="I18" s="23">
         <f t="shared" si="4"/>
-        <v>64400</v>
+        <v>1513000</v>
       </c>
       <c r="J18" s="23">
         <f t="shared" si="4"/>
-        <v>63700</v>
+        <v>1496000</v>
       </c>
       <c r="K18" s="23">
         <f t="shared" si="4"/>
-        <v>160200</v>
+        <v>860000</v>
       </c>
       <c r="L18" s="23">
         <f t="shared" si="4"/>
-        <v>202400</v>
+        <v>892500</v>
       </c>
       <c r="M18" s="23">
         <f t="shared" si="4"/>
-        <v>200100</v>
-      </c>
-      <c r="N18" s="23">
-        <f>N16-N12</f>
-        <v>197800</v>
-      </c>
-      <c r="O18" s="20">
-        <f>O16-O12</f>
-        <v>617200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="23">
-        <f>B18</f>
-        <v>110000</v>
-      </c>
-      <c r="C19" s="23">
-        <f t="shared" ref="C19:M19" si="5">C18</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="23">
-        <f t="shared" si="5"/>
-        <v>-117600</v>
-      </c>
-      <c r="E19" s="23">
-        <f t="shared" si="5"/>
-        <v>-48000</v>
-      </c>
-      <c r="F19" s="23">
-        <f t="shared" si="5"/>
-        <v>-66500</v>
-      </c>
-      <c r="G19" s="23">
-        <f t="shared" si="5"/>
-        <v>-47000</v>
-      </c>
-      <c r="H19" s="23">
-        <f t="shared" si="5"/>
-        <v>-102300</v>
-      </c>
-      <c r="I19" s="23">
-        <f t="shared" si="5"/>
-        <v>64400</v>
-      </c>
-      <c r="J19" s="23">
-        <f t="shared" si="5"/>
-        <v>63700</v>
-      </c>
-      <c r="K19" s="23">
-        <f t="shared" si="5"/>
-        <v>160200</v>
-      </c>
-      <c r="L19" s="23">
-        <f t="shared" si="5"/>
-        <v>202400</v>
-      </c>
-      <c r="M19" s="23">
-        <f t="shared" si="5"/>
-        <v>200100</v>
-      </c>
-      <c r="N19" s="24">
-        <f>D19+N18</f>
-        <v>80200</v>
-      </c>
-      <c r="O19" s="17"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
+        <v>871500</v>
+      </c>
+      <c r="N18" s="24">
+        <f>D18+N17</f>
+        <v>211099.99999999988</v>
+      </c>
+      <c r="O18" s="17"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="3">
-        <f>(O16-O12)/O12</f>
-        <v>0.60056436703318083</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29" t="s">
+      <c r="B20" s="3">
+        <f>(O15-O11)/O11</f>
+        <v>1.2286827142868932</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="25" t="s">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+      <c r="E26" s="30"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B8:N8"/>
-    <mergeCell ref="B22:D22"/>
+  <mergeCells count="3">
+    <mergeCell ref="B7:N7"/>
     <mergeCell ref="A1:P1"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions gridLines="1"/>

</xml_diff>